<commit_message>
Scrape all profiles given in assignment
</commit_message>
<xml_diff>
--- a/Assignment.xlsx
+++ b/Assignment.xlsx
@@ -1,26 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keshav Chandak\OneDrive\Desktop\semester 8\Scaler\LinkedIn Scrapper\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6CDF836-A0F8-4E4A-B99F-69DC525A5374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -180,7 +169,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -210,20 +200,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="3">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -234,10 +227,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -264,82 +257,82 @@
         <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -351,402 +344,428 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
                 <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="9500"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot rev="0" lon="0" lat="0"/>
+            </a:camera>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:tint val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
   <dimension ref="A1:A50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="2" width="63.71928571428572" customWidth="1" bestFit="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18">
+      <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18">
+      <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18">
+      <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18">
+      <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18">
+      <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18">
+      <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18">
+      <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18">
+      <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18">
+      <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18">
+      <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18">
+      <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18">
+      <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18">
+      <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18">
+      <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18">
+      <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18">
+      <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18">
+      <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18">
+      <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18">
+      <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18">
+      <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18">
+      <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18">
+      <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18">
+      <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18">
+      <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18">
+      <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18">
+      <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18">
+      <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18">
+      <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18">
+      <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18">
+      <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18">
+      <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18">
+      <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18">
+      <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18">
+      <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18">
+      <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18">
+      <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18">
+      <c r="A48" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18">
+      <c r="A49" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18">
+      <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>